<commit_message>
update for remote CNOT
</commit_message>
<xml_diff>
--- a/result/QASM.xlsx
+++ b/result/QASM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\Anaconda3\Lib\site-packages\circuittransform\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FDD257-A845-4F70-8F88-01FF051584A9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476C08A6-2C2A-4F1B-BF9F-ED19F0C47828}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3546" yWindow="1379" windowWidth="17425" windowHeight="9052" xr2:uid="{A4679066-D772-4BC4-955E-CB79E73092DB}"/>
+    <workbookView minimized="1" xWindow="3667" yWindow="2469" windowWidth="17425" windowHeight="9051" xr2:uid="{A4679066-D772-4BC4-955E-CB79E73092DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -112,11 +112,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>[1, 0.5, 0.1]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>[1, 0.7, 0.2]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[1, 0.8, 0.6, 0.4]</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -505,7 +505,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
@@ -516,7 +516,7 @@
     <col min="7" max="7" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -690,10 +690,10 @@
         <v>641</v>
       </c>
       <c r="I8">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="J8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -739,7 +739,7 @@
         <v>812</v>
       </c>
       <c r="J10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add annealing search for initial mapping
</commit_message>
<xml_diff>
--- a/result/QASM.xlsx
+++ b/result/QASM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\Anaconda3\Lib\site-packages\circuittransform\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D7D83C-6F4D-46FB-872F-214BD431D4AB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B94216-D51E-4349-87DC-B4C634E44183}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4017" yWindow="1198" windowWidth="17426" windowHeight="9051" xr2:uid="{A4679066-D772-4BC4-955E-CB79E73092DB}"/>
+    <workbookView xWindow="1985" yWindow="1706" windowWidth="17425" windowHeight="9052" xr2:uid="{A4679066-D772-4BC4-955E-CB79E73092DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
   <si>
     <t>QASM</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -141,6 +141,38 @@
   </si>
   <si>
     <t>rd84_142</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>rd73_140</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>rd53_311</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>squar5_261</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sym9_146</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>比较</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>my method lookahead 1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>my method lookahead 2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>annealing for initial map</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -526,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99136C82-9D3C-4FB5-8521-8F896A17592B}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
@@ -539,12 +571,15 @@
     <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.109375" customWidth="1"/>
+    <col min="11" max="12" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.5546875" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -570,16 +605,25 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="J1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -598,8 +642,12 @@
       <c r="I2">
         <v>723</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <f>G2-I2</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -624,11 +672,21 @@
       <c r="I3">
         <v>536</v>
       </c>
-      <c r="K3" t="s">
+      <c r="J3">
+        <f t="shared" ref="J3:J21" si="0">G3-I3</f>
+        <v>101</v>
+      </c>
+      <c r="K3">
+        <v>438</v>
+      </c>
+      <c r="L3">
+        <v>459</v>
+      </c>
+      <c r="N3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -653,243 +711,438 @@
       <c r="I4">
         <v>816</v>
       </c>
-      <c r="K4" t="s">
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+      <c r="K4">
+        <v>651</v>
+      </c>
+      <c r="N4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <v>230</v>
+      </c>
+      <c r="C5">
+        <v>952</v>
+      </c>
+      <c r="F5">
+        <v>916</v>
+      </c>
+      <c r="G5">
+        <v>934</v>
+      </c>
+      <c r="I5">
+        <v>972</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>-38</v>
+      </c>
+      <c r="N5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6">
+        <v>275</v>
+      </c>
+      <c r="C6">
+        <v>1367</v>
+      </c>
+      <c r="F6">
+        <v>1044</v>
+      </c>
+      <c r="G6">
+        <v>1092</v>
+      </c>
+      <c r="I6">
+        <v>1148</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>-56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <v>328</v>
+      </c>
+      <c r="C7">
+        <v>1436</v>
+      </c>
+      <c r="F7">
+        <v>1240</v>
+      </c>
+      <c r="G7">
+        <v>1317</v>
+      </c>
+      <c r="I7">
+        <v>1472</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>-155</v>
+      </c>
+      <c r="K7">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="B5">
+      <c r="B8">
         <v>343</v>
       </c>
-      <c r="G5">
+      <c r="G8">
         <v>1381</v>
       </c>
-      <c r="J5">
+      <c r="I8">
+        <v>1339</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="M8">
         <v>457</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B9">
         <v>480</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C9" s="1">
         <v>235</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="F6" s="1">
+      <c r="D9" s="1"/>
+      <c r="F9" s="1">
         <v>235</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="G9" s="2">
+        <v>680</v>
+      </c>
+      <c r="I9" s="2">
+        <v>582</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>98</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>3</v>
       </c>
-      <c r="B7">
+      <c r="B10">
         <v>512</v>
       </c>
-      <c r="C7">
+      <c r="C10">
         <v>2193</v>
       </c>
-      <c r="F7">
+      <c r="F10">
         <v>1299</v>
       </c>
-      <c r="G7">
+      <c r="G10">
         <v>1776</v>
       </c>
-      <c r="I7">
+      <c r="I10">
         <v>1724</v>
       </c>
-      <c r="K7" t="s">
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="N10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B11">
         <v>986</v>
       </c>
-      <c r="C8">
+      <c r="C11">
         <v>3632</v>
       </c>
-      <c r="F8">
+      <c r="F11">
         <v>3176</v>
       </c>
-      <c r="G8">
+      <c r="G11">
         <v>3867</v>
       </c>
-      <c r="I8">
+      <c r="I11">
         <v>3292</v>
       </c>
-      <c r="K8" t="s">
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>575</v>
+      </c>
+      <c r="K11">
+        <v>2962</v>
+      </c>
+      <c r="N11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="B9">
+      <c r="B12">
         <v>1221</v>
       </c>
-      <c r="C9">
+      <c r="C12">
         <v>4254</v>
       </c>
-      <c r="F9">
+      <c r="F12">
         <v>4039</v>
       </c>
-      <c r="G9">
+      <c r="G12">
         <v>4528</v>
       </c>
-      <c r="I9">
+      <c r="I12">
         <v>3530</v>
       </c>
-      <c r="K9" t="s">
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>998</v>
+      </c>
+      <c r="N12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B10">
+      <c r="B13">
         <v>1776</v>
       </c>
-      <c r="C10">
+      <c r="C13">
         <v>6473</v>
       </c>
-      <c r="F10">
+      <c r="F13">
         <v>5572</v>
       </c>
-      <c r="G10">
+      <c r="G13">
         <v>6209</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="I13">
+        <v>5989</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14">
+        <v>1993</v>
+      </c>
+      <c r="C14">
+        <v>7948</v>
+      </c>
+      <c r="F14">
+        <v>6453</v>
+      </c>
+      <c r="G14">
+        <v>7348</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>7348</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B15">
         <v>3009</v>
       </c>
-      <c r="C11">
+      <c r="C15">
         <v>11921</v>
       </c>
-      <c r="F11">
+      <c r="F15">
         <v>10166</v>
       </c>
-      <c r="G11">
+      <c r="G15">
         <v>11340</v>
       </c>
-      <c r="I11">
-        <f>7838+B11</f>
+      <c r="I15">
+        <f>7838+B15</f>
         <v>10847</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>493</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>8</v>
       </c>
-      <c r="B12">
+      <c r="B16">
         <v>3073</v>
       </c>
-      <c r="C12">
+      <c r="C16">
         <v>12041</v>
       </c>
-      <c r="F12">
+      <c r="F16">
         <v>10002</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="G16">
+        <v>11193</v>
+      </c>
+      <c r="I16">
+        <v>10704</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>489</v>
+      </c>
+      <c r="N16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>24</v>
       </c>
-      <c r="B13">
+      <c r="B17">
         <v>3888</v>
       </c>
-      <c r="G13">
+      <c r="G17">
         <v>13426</v>
       </c>
-      <c r="I13">
+      <c r="I17">
         <v>11913</v>
       </c>
-      <c r="K13" t="s">
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>1513</v>
+      </c>
+      <c r="N17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B14">
+      <c r="B18">
         <v>10223</v>
       </c>
-      <c r="C14">
+      <c r="C18">
         <v>37781</v>
       </c>
-      <c r="E14">
+      <c r="E18">
         <v>42134</v>
       </c>
-      <c r="F14">
+      <c r="F18">
         <v>32009</v>
       </c>
-      <c r="G14">
+      <c r="G18">
         <v>36957</v>
       </c>
-      <c r="H14">
+      <c r="H18">
         <v>36635</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>36957</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B19">
         <v>27126</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C19" t="s">
         <v>15</v>
       </c>
-      <c r="F15">
+      <c r="F19">
         <v>86049</v>
       </c>
-      <c r="G15">
+      <c r="G19">
         <v>96852</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>96852</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>16</v>
       </c>
-      <c r="B16">
+      <c r="B20">
         <v>207775</v>
       </c>
-      <c r="C16">
+      <c r="C20">
         <v>743973</v>
       </c>
-      <c r="E16">
+      <c r="E20">
         <v>824792</v>
       </c>
-      <c r="F16">
+      <c r="F20">
         <v>653249</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="I1:I15" xr:uid="{EF70D8E8-481A-4035-A238-8E1AD3478CB8}"/>
-  <sortState ref="A2:K16">
-    <sortCondition ref="B2:B16"/>
+  <sortState ref="A2:N22">
+    <sortCondition ref="B2:B22"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="J1:K1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>